<commit_message>
Adding files for location recognition
</commit_message>
<xml_diff>
--- a/data/completo/TestPrecision.xlsx
+++ b/data/completo/TestPrecision.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NoGravity" sheetId="1" r:id="rId1"/>
@@ -740,6 +740,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -773,44 +809,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +930,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1250,11 +1249,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-496981536"/>
-        <c:axId val="-496988064"/>
+        <c:axId val="-342441728"/>
+        <c:axId val="-342440096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-496981536"/>
+        <c:axId val="-342441728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1295,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-496988064"/>
+        <c:crossAx val="-342440096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1304,7 +1303,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-496988064"/>
+        <c:axId val="-342440096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1352,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-496981536"/>
+        <c:crossAx val="-342441728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1465,7 +1464,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1785,11 +1783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-496976640"/>
-        <c:axId val="-496976096"/>
+        <c:axId val="-342434112"/>
+        <c:axId val="-342434656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-496976640"/>
+        <c:axId val="-342434112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1829,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-496976096"/>
+        <c:crossAx val="-342434656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1839,7 +1837,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-496976096"/>
+        <c:axId val="-342434656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,7 +1886,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-496976640"/>
+        <c:crossAx val="-342434112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2316,11 +2314,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="100"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2825,24 +2823,24 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="90"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
+      <c r="B24" s="102"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36"/>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="88"/>
-      <c r="D25" s="89"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="101"/>
       <c r="E25" s="37"/>
       <c r="F25" s="38" t="s">
         <v>3</v>
@@ -3265,8 +3263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3584,22 +3582,22 @@
       <c r="G16" s="52"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="52"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="40"/>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="93"/>
+      <c r="C18" s="105"/>
       <c r="D18" s="47" t="s">
         <v>2</v>
       </c>
@@ -3621,7 +3619,10 @@
       <c r="C19" s="13">
         <v>33</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="14">
+        <f>(B19+C20) / SUM(B19:C20)</f>
+        <v>0.7822349570200573</v>
+      </c>
       <c r="E19" s="13">
         <v>0.84099999999999997</v>
       </c>
@@ -3657,7 +3658,10 @@
       <c r="C21" s="21">
         <v>23</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="22">
+        <f>(B21+C22) / SUM(B21:C22)</f>
+        <v>0.81904761904761902</v>
+      </c>
       <c r="E21" s="21">
         <v>0.86499999999999999</v>
       </c>
@@ -3844,7 +3848,7 @@
     <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;"Helvetica,Regular"&amp;11&amp;P</oddFooter>
   </headerFooter>
@@ -3871,11 +3875,11 @@
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95"/>
-      <c r="D1" s="96"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="108"/>
       <c r="E1" s="53" t="s">
         <v>2</v>
       </c>
@@ -4266,24 +4270,24 @@
       <c r="H19" s="57"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="97"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="109"/>
       <c r="H20" s="57"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="96"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="108"/>
       <c r="E21" s="10"/>
       <c r="F21" s="53" t="s">
         <v>3</v>
@@ -4705,8 +4709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4995,21 +4999,21 @@
       <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="90"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="90"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="29" t="s">
         <v>2</v>
       </c>
@@ -5030,7 +5034,10 @@
       <c r="C18" s="30">
         <v>24</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="31">
+        <f>(B18+C19) / SUM(B18:C19)</f>
+        <v>0.81764705882352939</v>
+      </c>
       <c r="E18" s="75">
         <v>0.85799999999999998</v>
       </c>
@@ -5064,7 +5071,10 @@
       <c r="C20" s="86">
         <v>41</v>
       </c>
-      <c r="D20" s="86"/>
+      <c r="D20" s="86">
+        <f>(B20+C21) / SUM(B20:C21)</f>
+        <v>0.75728155339805825</v>
+      </c>
       <c r="E20" s="86">
         <v>0.84499999999999997</v>
       </c>
@@ -5266,406 +5276,406 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="101" t="s">
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="F1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="101" t="s">
+      <c r="G1" s="87" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="101"/>
-      <c r="B2" s="103">
+      <c r="A2" s="87"/>
+      <c r="B2" s="88">
         <v>227</v>
       </c>
-      <c r="C2" s="103">
+      <c r="C2" s="88">
         <v>16</v>
       </c>
-      <c r="D2" s="103">
+      <c r="D2" s="88">
         <v>17</v>
       </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103">
+      <c r="E2" s="88"/>
+      <c r="F2" s="88">
         <v>0.86</v>
       </c>
-      <c r="G2" s="103">
+      <c r="G2" s="88">
         <v>0.873</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="103">
+      <c r="B3" s="88">
         <v>22</v>
       </c>
-      <c r="C3" s="103">
+      <c r="C3" s="88">
         <v>9</v>
       </c>
-      <c r="D3" s="103">
+      <c r="D3" s="88">
         <v>4</v>
       </c>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103">
+      <c r="E3" s="88"/>
+      <c r="F3" s="88">
         <v>0.36</v>
       </c>
-      <c r="G3" s="103">
+      <c r="G3" s="88">
         <v>0.25700000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106">
+      <c r="A4" s="90"/>
+      <c r="B4" s="91">
         <v>15</v>
       </c>
-      <c r="C4" s="106">
+      <c r="C4" s="91">
         <v>0</v>
       </c>
-      <c r="D4" s="106">
+      <c r="D4" s="91">
         <v>39</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106">
+      <c r="E4" s="91"/>
+      <c r="F4" s="91">
         <v>0.65</v>
       </c>
-      <c r="G4" s="106">
+      <c r="G4" s="91">
         <v>0.72199999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108">
+      <c r="A5" s="92"/>
+      <c r="B5" s="93">
         <v>216</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="93">
         <v>8</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="93">
         <v>17</v>
       </c>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108">
+      <c r="E5" s="93"/>
+      <c r="F5" s="93">
         <v>0.85699999999999998</v>
       </c>
-      <c r="G5" s="108">
+      <c r="G5" s="93">
         <v>0.89600000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="103">
+      <c r="B6" s="88">
         <v>21</v>
       </c>
-      <c r="C6" s="103">
+      <c r="C6" s="88">
         <v>6</v>
       </c>
-      <c r="D6" s="103">
+      <c r="D6" s="88">
         <v>4</v>
       </c>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103">
+      <c r="E6" s="88"/>
+      <c r="F6" s="88">
         <v>0.33300000000000002</v>
       </c>
-      <c r="G6" s="103">
+      <c r="G6" s="88">
         <v>0.19400000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="105"/>
-      <c r="B7" s="106">
+      <c r="A7" s="90"/>
+      <c r="B7" s="91">
         <v>15</v>
       </c>
-      <c r="C7" s="106">
+      <c r="C7" s="91">
         <v>4</v>
       </c>
-      <c r="D7" s="106">
+      <c r="D7" s="91">
         <v>24</v>
       </c>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106">
+      <c r="E7" s="91"/>
+      <c r="F7" s="91">
         <v>0.53300000000000003</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G7" s="91">
         <v>0.55800000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="107"/>
-      <c r="B8" s="108">
+      <c r="A8" s="92"/>
+      <c r="B8" s="93">
         <v>179</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="93">
         <v>3</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="93">
         <v>14</v>
       </c>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108">
+      <c r="E8" s="93"/>
+      <c r="F8" s="93">
         <v>0.873</v>
       </c>
-      <c r="G8" s="108">
+      <c r="G8" s="93">
         <v>0.91300000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="103">
+      <c r="B9" s="88">
         <v>13</v>
       </c>
-      <c r="C9" s="103">
+      <c r="C9" s="88">
         <v>9</v>
       </c>
-      <c r="D9" s="103">
+      <c r="D9" s="88">
         <v>2</v>
       </c>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103">
+      <c r="E9" s="88"/>
+      <c r="F9" s="88">
         <v>0.69199999999999995</v>
       </c>
-      <c r="G9" s="103">
+      <c r="G9" s="88">
         <v>0.375</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="105"/>
-      <c r="B10" s="106">
+      <c r="A10" s="90"/>
+      <c r="B10" s="91">
         <v>13</v>
       </c>
-      <c r="C10" s="106">
+      <c r="C10" s="91">
         <v>1</v>
       </c>
-      <c r="D10" s="106">
+      <c r="D10" s="91">
         <v>26</v>
       </c>
-      <c r="E10" s="106"/>
-      <c r="F10" s="106">
+      <c r="E10" s="91"/>
+      <c r="F10" s="91">
         <v>0.61899999999999999</v>
       </c>
-      <c r="G10" s="106">
+      <c r="G10" s="91">
         <v>0.65</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="107"/>
-      <c r="B11" s="108">
+      <c r="A11" s="92"/>
+      <c r="B11" s="93">
         <v>149</v>
       </c>
-      <c r="C11" s="108">
+      <c r="C11" s="93">
         <v>9</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D11" s="93">
         <v>8</v>
       </c>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108">
+      <c r="E11" s="93"/>
+      <c r="F11" s="93">
         <v>0.89800000000000002</v>
       </c>
-      <c r="G11" s="108">
+      <c r="G11" s="93">
         <v>0.89800000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="103">
+      <c r="B12" s="88">
         <v>11</v>
       </c>
-      <c r="C12" s="103">
+      <c r="C12" s="88">
         <v>18</v>
       </c>
-      <c r="D12" s="103">
+      <c r="D12" s="88">
         <v>4</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103">
+      <c r="E12" s="88"/>
+      <c r="F12" s="88">
         <v>0.66700000000000004</v>
       </c>
-      <c r="G12" s="103">
+      <c r="G12" s="88">
         <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="105"/>
-      <c r="B13" s="106">
+      <c r="A13" s="90"/>
+      <c r="B13" s="91">
         <v>6</v>
       </c>
-      <c r="C13" s="106">
+      <c r="C13" s="91">
         <v>0</v>
       </c>
-      <c r="D13" s="106">
+      <c r="D13" s="91">
         <v>4</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106">
+      <c r="E13" s="91"/>
+      <c r="F13" s="91">
         <v>0.25</v>
       </c>
-      <c r="G13" s="106">
+      <c r="G13" s="91">
         <v>0.308</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="107"/>
-      <c r="B14" s="108">
+      <c r="A14" s="92"/>
+      <c r="B14" s="93">
         <v>150</v>
       </c>
-      <c r="C14" s="108">
+      <c r="C14" s="93">
         <v>8</v>
       </c>
-      <c r="D14" s="108">
+      <c r="D14" s="93">
         <v>2</v>
       </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="108">
+      <c r="E14" s="93"/>
+      <c r="F14" s="93">
         <v>0.93799999999999994</v>
       </c>
-      <c r="G14" s="108">
+      <c r="G14" s="93">
         <v>0.93799999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="103">
+      <c r="B15" s="88">
         <v>7</v>
       </c>
-      <c r="C15" s="103">
+      <c r="C15" s="88">
         <v>18</v>
       </c>
-      <c r="D15" s="103">
+      <c r="D15" s="88">
         <v>0</v>
       </c>
-      <c r="E15" s="103"/>
-      <c r="F15" s="103">
+      <c r="E15" s="88"/>
+      <c r="F15" s="88">
         <v>0.69199999999999995</v>
       </c>
-      <c r="G15" s="103">
+      <c r="G15" s="88">
         <v>0.72</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="106">
+      <c r="A16" s="90"/>
+      <c r="B16" s="91">
         <v>3</v>
       </c>
-      <c r="C16" s="106">
+      <c r="C16" s="91">
         <v>0</v>
       </c>
-      <c r="D16" s="106">
+      <c r="D16" s="91">
         <v>3</v>
       </c>
-      <c r="E16" s="106"/>
-      <c r="F16" s="106">
+      <c r="E16" s="91"/>
+      <c r="F16" s="91">
         <v>0.6</v>
       </c>
-      <c r="G16" s="106">
+      <c r="G16" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="107"/>
-      <c r="B17" s="108">
+      <c r="A17" s="92"/>
+      <c r="B17" s="93">
         <v>117</v>
       </c>
-      <c r="C17" s="108">
+      <c r="C17" s="93">
         <v>2</v>
       </c>
-      <c r="D17" s="108">
+      <c r="D17" s="93">
         <v>4</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108">
+      <c r="E17" s="93"/>
+      <c r="F17" s="93">
         <v>0.93600000000000005</v>
       </c>
-      <c r="G17" s="108">
+      <c r="G17" s="93">
         <v>0.95099999999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="103">
+      <c r="B18" s="88">
         <v>7</v>
       </c>
-      <c r="C18" s="103">
+      <c r="C18" s="88">
         <v>11</v>
       </c>
-      <c r="D18" s="103">
+      <c r="D18" s="88">
         <v>1</v>
       </c>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103">
+      <c r="E18" s="88"/>
+      <c r="F18" s="88">
         <v>0.78600000000000003</v>
       </c>
-      <c r="G18" s="103">
+      <c r="G18" s="88">
         <v>0.57899999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="105"/>
-      <c r="B19" s="106">
+      <c r="A19" s="90"/>
+      <c r="B19" s="91">
         <v>1</v>
       </c>
-      <c r="C19" s="106">
+      <c r="C19" s="91">
         <v>1</v>
       </c>
-      <c r="D19" s="106">
+      <c r="D19" s="91">
         <v>2</v>
       </c>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106">
+      <c r="E19" s="91"/>
+      <c r="F19" s="91">
         <v>0.28599999999999998</v>
       </c>
-      <c r="G19" s="106">
+      <c r="G19" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="107"/>
-      <c r="B20" s="109"/>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5690,244 +5700,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="102"/>
-      <c r="D1" s="101" t="s">
+      <c r="C1" s="110"/>
+      <c r="D1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="F1" s="87" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="103">
+      <c r="B2" s="88">
         <v>235</v>
       </c>
-      <c r="C2" s="103">
+      <c r="C2" s="88">
         <v>25</v>
       </c>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103">
+      <c r="D2" s="88"/>
+      <c r="E2" s="88">
         <v>0.86399999999999999</v>
       </c>
-      <c r="F2" s="103">
+      <c r="F2" s="88">
         <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106">
+      <c r="A3" s="91"/>
+      <c r="B3" s="91">
         <v>37</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="91">
         <v>52</v>
       </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106">
+      <c r="D3" s="91"/>
+      <c r="E3" s="91">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F3" s="106">
+      <c r="F3" s="91">
         <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="93">
         <v>211</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="93">
         <v>30</v>
       </c>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108">
+      <c r="D4" s="93"/>
+      <c r="E4" s="93">
         <v>0.90200000000000002</v>
       </c>
-      <c r="F4" s="108">
+      <c r="F4" s="93">
         <v>0.876</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106">
+      <c r="A5" s="91"/>
+      <c r="B5" s="91">
         <v>23</v>
       </c>
-      <c r="C5" s="106">
+      <c r="C5" s="91">
         <v>51</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106">
+      <c r="D5" s="91"/>
+      <c r="E5" s="91">
         <v>0.63</v>
       </c>
-      <c r="F5" s="106">
+      <c r="F5" s="91">
         <v>0.68899999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="108">
+      <c r="B6" s="93">
         <v>175</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="93">
         <v>21</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108">
+      <c r="D6" s="93"/>
+      <c r="E6" s="93">
         <v>0.91100000000000003</v>
       </c>
-      <c r="F6" s="108">
+      <c r="F6" s="93">
         <v>0.89300000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106"/>
-      <c r="B7" s="106">
+      <c r="A7" s="91"/>
+      <c r="B7" s="91">
         <v>17</v>
       </c>
-      <c r="C7" s="106">
+      <c r="C7" s="91">
         <v>47</v>
       </c>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106">
+      <c r="D7" s="91"/>
+      <c r="E7" s="91">
         <v>0.69099999999999995</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F7" s="91">
         <v>0.73399999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="108">
+      <c r="B8" s="93">
         <v>153</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="93">
         <v>13</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108">
+      <c r="D8" s="93"/>
+      <c r="E8" s="93">
         <v>0.89</v>
       </c>
-      <c r="F8" s="108">
+      <c r="F8" s="93">
         <v>0.92200000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
-      <c r="B9" s="106">
+      <c r="A9" s="91"/>
+      <c r="B9" s="91">
         <v>19</v>
       </c>
-      <c r="C9" s="106">
+      <c r="C9" s="91">
         <v>24</v>
       </c>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106">
+      <c r="D9" s="91"/>
+      <c r="E9" s="91">
         <v>0.64900000000000002</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="91">
         <v>0.55800000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="93">
         <v>151</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="93">
         <v>9</v>
       </c>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108">
+      <c r="D10" s="93"/>
+      <c r="E10" s="93">
         <v>0.92600000000000005</v>
       </c>
-      <c r="F10" s="108">
+      <c r="F10" s="93">
         <v>0.94399999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="106"/>
-      <c r="B11" s="106">
+      <c r="A11" s="91"/>
+      <c r="B11" s="91">
         <v>12</v>
       </c>
-      <c r="C11" s="106">
+      <c r="C11" s="91">
         <v>19</v>
       </c>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106">
+      <c r="D11" s="91"/>
+      <c r="E11" s="91">
         <v>0.67900000000000005</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="91">
         <v>0.61299999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="108">
+      <c r="B12" s="93">
         <v>115</v>
       </c>
-      <c r="C12" s="108">
+      <c r="C12" s="93">
         <v>8</v>
       </c>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108">
+      <c r="D12" s="93"/>
+      <c r="E12" s="93">
         <v>0.94299999999999995</v>
       </c>
-      <c r="F12" s="108">
+      <c r="F12" s="93">
         <v>0.93500000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
-      <c r="B13" s="106">
+      <c r="A13" s="91"/>
+      <c r="B13" s="91">
         <v>7</v>
       </c>
-      <c r="C13" s="106">
+      <c r="C13" s="91">
         <v>16</v>
       </c>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106">
+      <c r="D13" s="91"/>
+      <c r="E13" s="91">
         <v>0.66700000000000004</v>
       </c>
-      <c r="F13" s="106">
+      <c r="F13" s="91">
         <v>0.69599999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="108"/>
-      <c r="C14" s="108"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="108"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="106"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>